<commit_message>
Bonds DV01, Duration - All 3 types, YTM
Bonds DV01, Duration - All 3 types, YTM
Interest Rate risk in Banking Book
</commit_message>
<xml_diff>
--- a/Bonds_IRRBB.xlsx
+++ b/Bonds_IRRBB.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jobs_2021_2022\MORGAN_STANLEY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacka\OneDrive\Desktop\GITHUB_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBAC737-B5DB-4C08-AE70-08FACD94ACCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320C9F03-D21C-43D1-AF83-D9261C241947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bonds_IRRBB" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="IRRBB" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Time to Maturity (Years)</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>DV01</t>
+  </si>
+  <si>
+    <t>EVE is specifically used to measure banks’ IRRBB in a standardised outlier test, with supervisors entitled to take action if a bank experiences a change in EVE of more than 15% of common equity Tier 1 under the outlier test.</t>
+  </si>
+  <si>
+    <t>If rates were to increase and a bank’s deposits repriced sooner than its loans, it could result in the bank paying out more interest on deposits than the interest it is receiving from loans. The mismatch would subsequently bite into the bank’s net interest income, as well as affecting the economic value of its equity (EVE), which is derived by discounting future cash inflows and outflows.</t>
+  </si>
+  <si>
+    <t>Interest rate risk in the banking book is the risk posed by adverse movements in interest rates that cause a mismatch between the rates banks set on customer loans and on deposits.</t>
   </si>
 </sst>
 </file>
@@ -115,12 +124,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -215,9 +224,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -275,7 +284,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -293,11 +302,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -677,29 +689,29 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -718,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -726,7 +738,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -734,7 +746,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -760,7 +772,7 @@
       </c>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -789,7 +801,7 @@
         <v>1217.5123093736061</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -818,7 +830,7 @@
         <v>1140.6289581646822</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -847,7 +859,7 @@
         <v>1068.6006294862132</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -876,7 +888,7 @@
         <v>1001.1207388384262</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -905,7 +917,7 @@
         <v>937.90206189030414</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -931,7 +943,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>7</v>
       </c>
@@ -957,7 +969,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -982,7 +994,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="C15" s="13">
         <f>SUM(C7:C14)</f>
@@ -1000,7 +1012,7 @@
         <v>6.7404347977130294</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1008,7 +1020,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1073,7 +1085,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E19" s="22"/>
       <c r="F19" s="23"/>
       <c r="H19" s="24">
@@ -1104,7 +1116,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H20" s="24">
         <v>1E-4</v>
       </c>
@@ -1133,7 +1145,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E21" s="15" t="s">
         <v>23</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>6.6677706642561816</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
       <c r="H23" s="1" t="s">
         <v>24</v>
@@ -1163,7 +1175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E24" s="15" t="s">
         <v>26</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>66.899999999999864</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H25" s="24">
         <v>1E-3</v>
       </c>
@@ -1216,7 +1228,7 @@
         <v>6.6900000000000546</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H26" s="24">
         <v>1E-4</v>
       </c>
@@ -1239,14 +1251,14 @@
         <v>0.66899999999998272</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O29" s="28"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O30" s="28"/>
     </row>
   </sheetData>
@@ -1257,13 +1269,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43F8D2F-5891-4839-BB8E-CB8394B02431}">
+  <dimension ref="B2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="175.44140625" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>